<commit_message>
Added JS Array methods & Updated Tracking Sheet
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>Arithmetic Operators, Comparison Operators, Logical Operators</t>
+  </si>
+  <si>
+    <t>Strings, while loop, do-while loop</t>
   </si>
 </sst>
 </file>
@@ -313,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -331,7 +334,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,7 +1283,7 @@
       <c r="C53" s="3">
         <v>45338</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1310,24 +1312,28 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
+      <c r="A56" s="5"/>
       <c r="B56" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C56" s="3">
         <v>45341</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="2"/>
+      <c r="A57" s="4"/>
       <c r="B57" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C57" s="3">
         <v>45342</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>

</xml_diff>

<commit_message>
Date: 21-02-2024 (for loop, functions)
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Strings, while loop, do-while loop</t>
+  </si>
+  <si>
+    <t>Types of for loop, Types of functions</t>
   </si>
 </sst>
 </file>
@@ -616,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,14 +1339,16 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="2"/>
+      <c r="A58" s="4"/>
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="3">
         <v>45343</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="15" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>

</xml_diff>

<commit_message>
Date: 22-02-2024 (Arrow function, Callback Function)
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Types of for loop, Types of functions</t>
+  </si>
+  <si>
+    <t>Arrow function, Callback function</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1351,14 +1354,16 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
+      <c r="A59" s="4"/>
       <c r="B59" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C59" s="3">
         <v>45344</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="15" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>

</xml_diff>

<commit_message>
Introduction to TypeScript, RunTime Environment
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="60">
   <si>
     <t>Class Status</t>
   </si>
@@ -196,13 +196,19 @@
   </si>
   <si>
     <t>Nested Objects, Constructor Function, Class</t>
+  </si>
+  <si>
+    <t>Introduction to TypeScript, RunTime Environment</t>
+  </si>
+  <si>
+    <t>TypeScript</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,8 +235,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,8 +291,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -352,11 +383,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -427,6 +486,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -736,8 +812,8 @@
   </sheetPr>
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,10 +908,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
@@ -849,8 +925,10 @@
         <v>15</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
@@ -1708,27 +1786,31 @@
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="19"/>
+      <c r="A64" s="26"/>
       <c r="B64" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C64" s="9">
         <v>45349</v>
       </c>
-      <c r="D64" s="8"/>
+      <c r="D64" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
     </row>
     <row r="65" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="19"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="9">
         <v>45350</v>
       </c>
-      <c r="D65" s="8"/>
+      <c r="D65" s="32" t="s">
+        <v>58</v>
+      </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -2803,5 +2885,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Installation of Node & Typ
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="61">
   <si>
     <t>Class Status</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>TypeScript</t>
+  </si>
+  <si>
+    <t>Installation of node, Installation of typeScript</t>
   </si>
 </sst>
 </file>
@@ -813,7 +816,7 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1816,14 +1819,16 @@
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="19"/>
+      <c r="A66" s="27"/>
       <c r="B66" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C66" s="9">
         <v>45351</v>
       </c>
-      <c r="D66" s="8"/>
+      <c r="D66" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>

</xml_diff>

<commit_message>
TypeScript Configuration, Compilation Target version, Compilation of .ts file
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="62">
   <si>
     <t>Class Status</t>
   </si>
@@ -204,7 +204,10 @@
     <t>TypeScript</t>
   </si>
   <si>
-    <t>Installation of node, Installation of typeScript</t>
+    <t>TypeScript Configuration, Compilation Target version, Compilation of .ts file</t>
+  </si>
+  <si>
+    <t>Installation of Node, Installation of TypeScript</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,7 +827,7 @@
     <col min="1" max="1" width="10.6640625" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.5546875" style="24" bestFit="1" customWidth="1"/>
   </cols>
@@ -1827,47 +1830,53 @@
         <v>45351</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
     </row>
     <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="19"/>
+      <c r="A67" s="26"/>
       <c r="B67" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C67" s="9">
         <v>45352</v>
       </c>
-      <c r="D67" s="8"/>
+      <c r="D67" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="19"/>
+      <c r="A68" s="26"/>
       <c r="B68" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C68" s="9">
         <v>45353</v>
       </c>
-      <c r="D68" s="8"/>
+      <c r="D68" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
     </row>
     <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="19"/>
+      <c r="A69" s="27"/>
       <c r="B69" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C69" s="9">
         <v>45354</v>
       </c>
-      <c r="D69" s="8"/>
+      <c r="D69" s="32" t="s">
+        <v>60</v>
+      </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>

</xml_diff>

<commit_message>
DataTypes in TS, Return types of functions
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="63">
   <si>
     <t>Class Status</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Installation of Node, Installation of TypeScript</t>
+  </si>
+  <si>
+    <t>DataTypes in TS, Return types of functions</t>
   </si>
 </sst>
 </file>
@@ -819,7 +822,7 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1882,14 +1885,16 @@
       <c r="G69" s="4"/>
     </row>
     <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="19"/>
+      <c r="A70" s="27"/>
       <c r="B70" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C70" s="9">
         <v>45355</v>
       </c>
-      <c r="D70" s="8"/>
+      <c r="D70" s="32" t="s">
+        <v>62</v>
+      </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>

</xml_diff>

<commit_message>
Loops, Array, Tuple, Object, Enum, Union, Class
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="64">
   <si>
     <t>Class Status</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>DataTypes in TS, Return types of functions</t>
+  </si>
+  <si>
+    <t>Loops, Array, Tuple, Object, Enum, Union, Class</t>
   </si>
 </sst>
 </file>
@@ -822,7 +825,7 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1900,14 +1903,16 @@
       <c r="G70" s="4"/>
     </row>
     <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="19"/>
+      <c r="A71" s="27"/>
       <c r="B71" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C71" s="9">
         <v>45356</v>
       </c>
-      <c r="D71" s="8"/>
+      <c r="D71" s="32" t="s">
+        <v>63</v>
+      </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>

</xml_diff>

<commit_message>
2024-03-24: Angular folder structure
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="70">
   <si>
     <t>Class Status</t>
   </si>
@@ -229,13 +229,16 @@
   </si>
   <si>
     <t>Angular</t>
+  </si>
+  <si>
+    <t>Angular component folder structure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +274,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -590,13 +599,13 @@
     <xf numFmtId="3" fontId="2" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -907,7 +916,7 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2084,7 +2093,7 @@
       <c r="C77" s="42">
         <v>45362</v>
       </c>
-      <c r="D77" s="45" t="s">
+      <c r="D77" s="47" t="s">
         <v>67</v>
       </c>
       <c r="E77" s="4"/>
@@ -2167,14 +2176,14 @@
       <c r="G82" s="4"/>
     </row>
     <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="47"/>
+      <c r="A83" s="46"/>
       <c r="B83" s="38" t="s">
         <v>17</v>
       </c>
       <c r="C83" s="39">
         <v>45368</v>
       </c>
-      <c r="D83" s="46" t="s">
+      <c r="D83" s="45" t="s">
         <v>15</v>
       </c>
       <c r="E83" s="4"/>
@@ -2182,14 +2191,16 @@
       <c r="G83" s="4"/>
     </row>
     <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="19"/>
+      <c r="A84" s="27"/>
       <c r="B84" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C84" s="9">
         <v>45369</v>
       </c>
-      <c r="D84" s="8"/>
+      <c r="D84" s="47" t="s">
+        <v>69</v>
+      </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>

</xml_diff>

<commit_message>
Created first Angular component
</commit_message>
<xml_diff>
--- a/Course-Tracking-Sheet.xlsx
+++ b/Course-Tracking-Sheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="71">
   <si>
     <t>Class Status</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Angular component folder structure</t>
+  </si>
+  <si>
+    <t>First component created</t>
   </si>
 </sst>
 </file>
@@ -916,7 +919,7 @@
   <dimension ref="A1:G147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D84" sqref="D84"/>
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2206,14 +2209,16 @@
       <c r="G84" s="4"/>
     </row>
     <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="19"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C85" s="9">
         <v>45370</v>
       </c>
-      <c r="D85" s="8"/>
+      <c r="D85" s="47" t="s">
+        <v>70</v>
+      </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>

</xml_diff>